<commit_message>
fix caching in vignette
</commit_message>
<xml_diff>
--- a/vignettes/Alameda-May4-v1 output.xlsx
+++ b/vignettes/Alameda-May4-v1 output.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="356">
   <si>
     <t xml:space="preserve">date</t>
   </si>
@@ -86,10 +86,226 @@
     <t xml:space="preserve">$all.params</t>
   </si>
   <si>
+    <t xml:space="preserve">       r0.initial latent.period illness.length.given.nonhosp prop.hospitalized</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    1:   2.890940             4                            4        0.04202709</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    2:   2.443608             1                            5        0.06810695</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    3:   3.705172             3                            4        0.03828022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    4:   3.097102             2                            5        0.02517421</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    5:   4.921586             3                            7        0.03643845</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   ---                                                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 9996:   3.377879             2                            5        0.03032866</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 9997:   2.929420             4                            5        0.04777166</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 9998:   4.067994             4                            4        0.04787753</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 9999:   3.812798             4                            4        0.05059497</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10000:   3.143115             3                            4        0.01616573</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       hosp.length.of.stay  prop.icu prop.vent intervention1.date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    1:                  11 0.4487887 0.8292936         2020-03-07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    2:                  13 0.5502658 0.8831492         2020-03-07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    3:                  11 0.4664154 0.8195063         2020-03-07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    4:                   8 0.4287021 0.8479070         2020-03-07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    5:                  11 0.4736474 0.8533035         2020-03-07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   ---                                                           </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 9996:                  11 0.4393939 0.8796800         2020-03-07</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 9997:                   8 0.4920944 0.8337167         2020-03-07</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 9998:                  11 0.4706050 0.8279167         2020-03-07</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 9999:                   7 0.4675072 0.8122769         2020-03-07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10000:                  11 0.4511491 0.8924137         2020-03-07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       intervention1.multiplier intervention1.smooth.days intervention2.date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    1:                0.5251996                         5         2020-03-17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    2:                0.6580592                         5         2020-03-17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    3:                0.7779575                         5         2020-03-17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    4:                0.8273989                         7         2020-03-17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    5:                0.5157291                         8         2020-03-17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   ---                                                                      </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 9996:                0.8397557                         5         2020-03-17</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 9997:                0.4330270                         9         2020-03-17</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 9998:                0.6462548                         9         2020-03-17</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 9999:                0.5661305                         4         2020-03-17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10000:                0.4177203                         7         2020-03-17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       intervention2.multiplier intervention2.smooth.days intervention3.date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    1:                0.3952299                         8         2020-06-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    2:                0.4654842                         7         2020-06-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    3:                0.3139963                         5         2020-06-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    4:                0.5594182                         5         2020-06-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    5:                0.6443424                         6         2020-06-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 9996:                0.2966097                         6         2020-06-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 9997:                0.4457069                         8         2020-06-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 9998:                0.5541582                         5         2020-06-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 9999:                0.3275438                         7         2020-06-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10000:                0.9422704                         7         2020-06-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       intervention3.multiplier intervention3.smooth.days</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    1:                 1.679144                         7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    2:                 1.365394                         8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    3:                 1.471412                         5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    4:                 2.040386                        10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    5:                 1.449264                         7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   ---                                                   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 9996:                 1.541516                         4</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 9997:                 1.462749                         7</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 9998:                 1.414118                         5</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 9999:                 2.013811                         7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10000:                 1.605697                         5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       patients.in.hosp.are.infectious use.hosp.rate exposed.to.hospital</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    1:                           FALSE          TRUE                  10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    2:                           FALSE         FALSE                   8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    3:                            TRUE          TRUE                   6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    4:                            TRUE          TRUE                   8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    5:                            TRUE         FALSE                   8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   ---                                                                  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 9996:                            TRUE         FALSE                   9</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 9997:                            TRUE         FALSE                  10</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 9998:                            TRUE          TRUE                  11</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 9999:                           FALSE         FALSE                  10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10000:                            TRUE          TRUE                   9</t>
+  </si>
+  <si>
     <t xml:space="preserve">$devlist</t>
   </si>
   <si>
-    <t xml:space="preserve">NULL</t>
+    <t xml:space="preserve">quartz_off_screen </t>
+  </si>
+  <si>
+    <t xml:space="preserve">                2 </t>
   </si>
   <si>
     <t xml:space="preserve">$extras</t>
@@ -98,19 +314,391 @@
     <t xml:space="preserve">$extras$`Parameters with Distributions`</t>
   </si>
   <si>
+    <t xml:space="preserve">                      internal.name</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1:                   weight.labels</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2:               parameter.weights</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 3:                      r0.initial</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 4:                   latent.period</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 5:    illness.length.given.nonhosp</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 6:          infectious.to.hospital</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 7:               prop.hospitalized</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 8:             hosp.length.of.stay</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 9:                        prop.icu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10:                       prop.vent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11:              intervention1.date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12:        intervention1.multiplier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13:       intervention1.smooth.days</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14:              intervention2.date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15:        intervention2.multiplier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16:       intervention2.smooth.days</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17:              intervention3.date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18:        intervention3.multiplier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19:       intervention3.smooth.days</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20: patients.in.hosp.are.infectious</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21:                   use.hosp.rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                                              external.name</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1:                                                                    &lt;NA&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2:                                                                  Priors</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 3:                       Basic reproductive number R0 before Intervention1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 4:    Number of Days from Infection to Becoming Infectious (Latent Period)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 5:                                       Duration of infectiousness (days)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 6:             Time from onset of infectiousness to hospitalization (days)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 7:                               Percent of Infected that are Hospitalized</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 8:                                  Average Hospital Length of Stay (Days)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 9: Percent of Hospitalized COVID-19 Patients That are Currently in the ICU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10:    Percent of COVID-19 Patients in the ICU who are Currently Ventilated</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11:                                              Date of first intervention</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12:                                                           Re multiplier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13:                                                    Days to reach new Re</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14:                                             Date of second intervention</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15:                                                           Re multiplier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16:                                                    Days to reach new Re</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17:                                              Date of third intervention</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18:                                                           Re multiplier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19:                                                    Days to reach new Re</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20:                                     Patients in hospital are infectious</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21:   Contant rate to hospital (if FALSE, fixed number of days to hospital)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           low     midlow                 mid    midhigh       high</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1:         NA         NA User's "Best Guess"         NA         NA</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2:       0.05       0.15                 0.6       0.15       0.05</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 3:        2.5          3                 3.5          4        4.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 4:          0          2                   3          4          5</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 5:          3          4                   5          6          7</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 6:          4          5                   6          7          8</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 7:       0.01       0.02                0.04       0.05       0.06</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 8:          6          8                  10         12         14</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 9:        0.4       0.42                0.45       0.52       0.55</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10:        0.8       0.82                0.85       0.87        0.9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11: 2020-03-07 2020-03-07          2020-03-07 2020-03-07 2020-03-07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12:        0.4        0.5                 0.6        0.8          1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13:          3          5                   7          9         11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14: 2020-03-17 2020-03-17          2020-03-17 2020-03-17 2020-03-17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15:        0.3        0.4                0.45        0.8          1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16:          3          5                   7          9         11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17: 2020-06-01 2020-06-01          2020-06-01 2020-06-01 2020-06-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18:        1.1        1.2                 1.5        1.7          2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19:          3          5                   7          9         11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20:      FALSE      FALSE                TRUE      FALSE      FALSE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21:      FALSE      FALSE                TRUE      FALSE      FALSE</t>
+  </si>
+  <si>
     <t xml:space="preserve">$extras$`Model Inputs`</t>
   </si>
   <si>
+    <t xml:space="preserve">        internal.name            external.name      value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1:   total.population Number of People in Area    1671000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2: start.display.date    Projection Start Date 2020-03-15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3:           end.date      Projection End Date 2020-07-01</t>
+  </si>
+  <si>
     <t xml:space="preserve">$extras$`Hospitilization Data`</t>
   </si>
   <si>
+    <t xml:space="preserve">          Date LowerBound UpperBound</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1: 2020-04-01         52      59.80</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2: 2020-04-02         57      65.55</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 3: 2020-04-03         64      73.60</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 4: 2020-04-04         60      69.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 5: 2020-04-05         72      82.80</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 6: 2020-04-06         79      90.85</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 7: 2020-04-07         76      87.40</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 8: 2020-04-08         84      96.60</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 9: 2020-04-09         80      92.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10: 2020-04-10         93     106.95</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11: 2020-04-11         87     100.05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12: 2020-04-12         91     104.65</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13: 2020-04-13         85      97.75</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14: 2020-04-14         92     105.80</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15: 2020-04-15         81      93.15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16: 2020-04-16         73      83.95</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17: 2020-04-17         85      97.75</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18: 2020-04-18         82      94.30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19: 2020-04-19         84      96.60</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20: 2020-04-20         85      97.75</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21: 2020-04-21         85      97.75</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22: 2020-04-22         84      96.60</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23: 2020-04-23         81      93.15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24: 2020-04-24         79      90.85</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25: 2020-04-25         83      95.45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26: 2020-04-26         84      96.60</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27: 2020-04-27         81      93.15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">28: 2020-04-28         76      87.40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">29: 2020-04-29         76      87.40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30: 2020-04-30         74      85.10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">31: 2020-05-01         75      86.25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">32: 2020-05-02         73      83.95</t>
+  </si>
+  <si>
+    <t xml:space="preserve">33: 2020-05-03         73      83.95</t>
+  </si>
+  <si>
     <t xml:space="preserve">$extras$Internal</t>
   </si>
   <si>
+    <t xml:space="preserve">                    internal.name             value</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1:               search.max.iter                20</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2:               search.expander                 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 3:           search.num.init.exp                 9</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 4:               max.nonconverge              0.01</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 5:                   random.seed             12345</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 6:                output.filestr                NA</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 7:      add.timestamp.to.filestr             FALSE</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 8:           min.obs.date.to.fit                NA</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 9:           max.obs.date.to.fit                NA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10:               main.iterations             10000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11:         simulation.start.date        2020-01-23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12:        lower.bound.multiplier               0.9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13:        upper.bound.multiplier               1.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14:            required.in.bounds                 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15:                 show.progress              TRUE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16:  plot.observed.data.long.term             FALSE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17: plot.observed.data.short.term              TRUE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18:             lower.bound.label Confirmed COVID19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19:             upper.bound.label  Probable COVID19</t>
+  </si>
+  <si>
     <t xml:space="preserve">$extras$time.of.run</t>
   </si>
   <si>
-    <t xml:space="preserve">[1] "2020-05-07 10:47:02"</t>
+    <t xml:space="preserve">[1] "2020-05-07 13:53:24"</t>
   </si>
   <si>
     <t xml:space="preserve">$extras$LEMMA.version</t>
@@ -125,6 +713,108 @@
     <t xml:space="preserve">$hosp.bounds</t>
   </si>
   <si>
+    <t xml:space="preserve">          date lower  upper</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1: 2020-04-01    52  59.80</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2: 2020-04-02    57  65.55</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 3: 2020-04-03    64  73.60</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 4: 2020-04-04    60  69.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 5: 2020-04-05    72  82.80</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 6: 2020-04-06    79  90.85</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 7: 2020-04-07    76  87.40</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 8: 2020-04-08    84  96.60</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 9: 2020-04-09    80  92.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10: 2020-04-10    93 106.95</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11: 2020-04-11    87 100.05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12: 2020-04-12    91 104.65</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13: 2020-04-13    85  97.75</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14: 2020-04-14    92 105.80</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15: 2020-04-15    81  93.15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16: 2020-04-16    73  83.95</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17: 2020-04-17    85  97.75</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18: 2020-04-18    82  94.30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19: 2020-04-19    84  96.60</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20: 2020-04-20    85  97.75</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21: 2020-04-21    85  97.75</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22: 2020-04-22    84  96.60</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23: 2020-04-23    81  93.15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24: 2020-04-24    79  90.85</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25: 2020-04-25    83  95.45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26: 2020-04-26    84  96.60</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27: 2020-04-27    81  93.15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">28: 2020-04-28    76  87.40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">29: 2020-04-29    76  87.40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30: 2020-04-30    74  85.10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">31: 2020-05-01    75  86.25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">32: 2020-05-02    73  83.95</t>
+  </si>
+  <si>
+    <t xml:space="preserve">33: 2020-05-03    73  83.95</t>
+  </si>
+  <si>
     <t xml:space="preserve">$internal.args</t>
   </si>
   <si>
@@ -257,7 +947,145 @@
     <t xml:space="preserve">$observed.data</t>
   </si>
   <si>
+    <t xml:space="preserve">          date   hosp</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1: 2020-04-01 55.900</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2: 2020-04-02 61.275</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 3: 2020-04-03 68.800</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 4: 2020-04-04 64.500</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 5: 2020-04-05 77.400</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 6: 2020-04-06 84.925</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 7: 2020-04-07 81.700</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 8: 2020-04-08 90.300</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 9: 2020-04-09 86.000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10: 2020-04-10 99.975</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11: 2020-04-11 93.525</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12: 2020-04-12 97.825</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13: 2020-04-13 91.375</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14: 2020-04-14 98.900</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15: 2020-04-15 87.075</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16: 2020-04-16 78.475</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17: 2020-04-17 91.375</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18: 2020-04-18 88.150</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19: 2020-04-19 90.300</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20: 2020-04-20 91.375</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21: 2020-04-21 91.375</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22: 2020-04-22 90.300</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23: 2020-04-23 87.075</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24: 2020-04-24 84.925</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25: 2020-04-25 89.225</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26: 2020-04-26 90.300</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27: 2020-04-27 87.075</t>
+  </si>
+  <si>
+    <t xml:space="preserve">28: 2020-04-28 81.700</t>
+  </si>
+  <si>
+    <t xml:space="preserve">29: 2020-04-29 81.700</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30: 2020-04-30 79.550</t>
+  </si>
+  <si>
+    <t xml:space="preserve">31: 2020-05-01 80.625</t>
+  </si>
+  <si>
+    <t xml:space="preserve">32: 2020-05-02 78.475</t>
+  </si>
+  <si>
+    <t xml:space="preserve">33: 2020-05-03 78.475</t>
+  </si>
+  <si>
     <t xml:space="preserve">$upp.params</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   r0.initial latent.period illness.length.given.nonhosp prop.hospitalized</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1:        3.5             3                            5              0.04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   hosp.length.of.stay prop.icu prop.vent intervention1.date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1:                  10     0.45      0.85         2020-03-07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   intervention1.multiplier intervention1.smooth.days intervention2.date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1:                      0.6                         7         2020-03-17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   intervention2.multiplier intervention2.smooth.days intervention3.date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1:                     0.45                         7         2020-06-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   intervention3.multiplier intervention3.smooth.days</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1:                      1.5                         7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   patients.in.hosp.are.infectious use.hosp.rate exposed.to.hospital</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1:                            TRUE          TRUE                   9</t>
   </si>
 </sst>
 </file>
@@ -15133,486 +15961,1901 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>20</v>
+        <v>48</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>20</v>
+        <v>51</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>20</v>
+        <v>54</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>20</v>
+        <v>57</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>20</v>
+        <v>60</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>20</v>
+        <v>63</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>20</v>
+        <v>65</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>50</v>
+        <v>66</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>20</v>
+        <v>68</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>52</v>
+        <v>69</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>51</v>
+        <v>70</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>20</v>
+        <v>71</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>53</v>
+        <v>72</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>54</v>
+        <v>73</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>20</v>
+        <v>74</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>55</v>
+        <v>75</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>56</v>
+        <v>76</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>20</v>
+        <v>77</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>57</v>
+        <v>78</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>58</v>
+        <v>79</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>20</v>
+        <v>80</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>59</v>
+        <v>81</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>60</v>
+        <v>82</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>20</v>
+        <v>83</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>61</v>
+        <v>84</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>20</v>
+        <v>86</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>63</v>
+        <v>87</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>64</v>
+        <v>88</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>20</v>
+        <v>89</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>65</v>
+        <v>90</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>49</v>
+        <v>91</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>20</v>
+        <v>92</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>66</v>
+        <v>20</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>64</v>
+        <v>93</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>20</v>
+        <v>94</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>67</v>
+        <v>95</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>68</v>
+        <v>20</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>20</v>
+        <v>96</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>69</v>
+        <v>97</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>70</v>
+        <v>98</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>20</v>
+        <v>99</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="s">
-        <v>20</v>
+        <v>100</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="s">
-        <v>71</v>
+        <v>101</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="s">
-        <v>72</v>
+        <v>102</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="s">
-        <v>73</v>
+        <v>103</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="s">
-        <v>20</v>
+        <v>104</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="s">
-        <v>74</v>
+        <v>105</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="s">
-        <v>75</v>
+        <v>106</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="s">
-        <v>20</v>
+        <v>107</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="s">
-        <v>76</v>
+        <v>108</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="s">
-        <v>77</v>
+        <v>109</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="s">
-        <v>20</v>
+        <v>110</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="s">
-        <v>20</v>
+        <v>111</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="s">
-        <v>78</v>
+        <v>112</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="s">
-        <v>20</v>
+        <v>113</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="s">
-        <v>79</v>
+        <v>114</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="293">
+      <c r="A293" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>